<commit_message>
EC1: UMCE results fully processed. Other classifiers' reports updated to add result category '27', which appeared only on UMCE.
</commit_message>
<xml_diff>
--- a/EC1-ECG_Analysis/ecg_oversampling/safetyArtist/Classifiers Conclusions Meanings.xlsx
+++ b/EC1-ECG_Analysis/ecg_oversampling/safetyArtist/Classifiers Conclusions Meanings.xlsx
@@ -10,14 +10,14 @@
     <sheet name="Classifiers Conclusion Meanings" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Classifiers Conclusion Meanings'!$A$1:$E$38</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Classifiers Conclusion Meanings'!$A$1:$E$39</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="21">
   <si>
     <t>NC</t>
   </si>
@@ -103,12 +103,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="5">
@@ -177,28 +183,28 @@
   </cellStyleXfs>
   <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -505,10 +511,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:E38"/>
+  <dimension ref="A1:E39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:C1"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -517,504 +523,518 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="1" t="s">
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="5" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" s="2">
+      <c r="B2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="2">
+      <c r="B3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" s="2">
+      <c r="B4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="1">
         <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" s="2">
+      <c r="B5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="1">
         <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6" s="2">
+      <c r="B6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="1">
         <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D7" s="2">
+      <c r="B7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="1">
         <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D8" s="2">
+      <c r="B8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="1">
         <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D9" s="2">
+      <c r="A9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" s="1">
         <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C10" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D10" s="2">
+      <c r="C10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" s="1">
         <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C11" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D11" s="2">
+      <c r="C11" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" s="1">
         <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C12" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D12" s="2">
+      <c r="C12" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" s="1">
         <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
+      <c r="A13" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C13" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D13" s="2">
+      <c r="C13" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13" s="1">
         <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
+      <c r="A14" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C14" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D14" s="2">
+      <c r="C14" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D14" s="1">
         <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
+      <c r="A15" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B15" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D15" s="2">
+      <c r="B15" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D15" s="1">
         <v>13</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
+      <c r="A16" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B16" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D16" s="2">
+      <c r="B16" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D16" s="1">
         <v>14</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
+      <c r="A17" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B17" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C17" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D17" s="2">
+      <c r="C17" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D17" s="1">
         <v>15</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
+      <c r="A18" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B18" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C18" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D18" s="2">
+      <c r="C18" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D18" s="1">
         <v>16</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
+      <c r="A19" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B19" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D19" s="2">
+      <c r="B19" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D19" s="1">
         <v>17</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
+      <c r="A20" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B20" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D20" s="2">
+      <c r="B20" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D20" s="1">
         <v>18</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
+      <c r="A21" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B21" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C21" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D21" s="2">
+      <c r="C21" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D21" s="1">
         <v>19</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D22" s="2">
+      <c r="A22" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D22" s="1">
         <v>20</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
+      <c r="A23" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="B23" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C23" s="2" t="s">
+      <c r="C23" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D23" s="2">
+      <c r="D23" s="1">
         <v>21</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="2" t="s">
+      <c r="A24" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="B24" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C24" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D24" s="2">
+      <c r="C24" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D24" s="1">
         <v>22</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="2" t="s">
+      <c r="A25" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="B25" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C25" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D25" s="2">
+      <c r="C25" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D25" s="1">
         <v>23</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="2" t="s">
+      <c r="A26" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="B26" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C26" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D26" s="2">
+      <c r="C26" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D26" s="1">
         <v>24</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="2" t="s">
+      <c r="A27" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B27" s="2" t="s">
+      <c r="B27" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C27" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D27" s="2">
+      <c r="C27" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D27" s="1">
         <v>25</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="2" t="s">
+      <c r="A28" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="B28" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C28" s="2" t="s">
+      <c r="C28" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D28" s="2">
+      <c r="D28" s="1">
         <v>26</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="1" t="s">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D29" s="1">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B30" s="6" t="s">
+      <c r="B31" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C30" s="7"/>
-      <c r="D30" s="7"/>
-      <c r="E30" s="8"/>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="2" t="s">
+      <c r="C31" s="7"/>
+      <c r="D31" s="7"/>
+      <c r="E31" s="8"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B31" s="4" t="s">
+      <c r="B32" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C31" s="4"/>
-      <c r="D31" s="4"/>
-      <c r="E31" s="4"/>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="2" t="s">
+      <c r="C32" s="3"/>
+      <c r="D32" s="3"/>
+      <c r="E32" s="3"/>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B32" s="4" t="s">
+      <c r="B33" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C32" s="4"/>
-      <c r="D32" s="4"/>
-      <c r="E32" s="4"/>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="2" t="s">
+      <c r="C33" s="3"/>
+      <c r="D33" s="3"/>
+      <c r="E33" s="3"/>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B33" s="5" t="s">
+      <c r="B34" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C33" s="5"/>
-      <c r="D33" s="5"/>
-      <c r="E33" s="5"/>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="2" t="s">
+      <c r="C34" s="2"/>
+      <c r="D34" s="2"/>
+      <c r="E34" s="2"/>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B34" s="5" t="s">
+      <c r="B35" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C34" s="5"/>
-      <c r="D34" s="5"/>
-      <c r="E34" s="5"/>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="2" t="s">
+      <c r="C35" s="2"/>
+      <c r="D35" s="2"/>
+      <c r="E35" s="2"/>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B35" s="5" t="s">
+      <c r="B36" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C35" s="5"/>
-      <c r="D35" s="5"/>
-      <c r="E35" s="5"/>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="2" t="s">
+      <c r="C36" s="2"/>
+      <c r="D36" s="2"/>
+      <c r="E36" s="2"/>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B36" s="5" t="s">
+      <c r="B37" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C36" s="5"/>
-      <c r="D36" s="5"/>
-      <c r="E36" s="5"/>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="2" t="s">
+      <c r="C37" s="2"/>
+      <c r="D37" s="2"/>
+      <c r="E37" s="2"/>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B37" s="5" t="s">
+      <c r="B38" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C37" s="5"/>
-      <c r="D37" s="5"/>
-      <c r="E37" s="5"/>
-    </row>
-    <row r="38" spans="1:5" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B38" s="5" t="s">
+      <c r="C38" s="2"/>
+      <c r="D38" s="2"/>
+      <c r="E38" s="2"/>
+    </row>
+    <row r="39" spans="1:5" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B39" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C38" s="5"/>
-      <c r="D38" s="5"/>
-      <c r="E38" s="5"/>
+      <c r="C39" s="2"/>
+      <c r="D39" s="2"/>
+      <c r="E39" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="B32:E32"/>
+    <mergeCell ref="B33:E33"/>
+    <mergeCell ref="B34:E34"/>
     <mergeCell ref="B35:E35"/>
     <mergeCell ref="B36:E36"/>
     <mergeCell ref="B37:E37"/>
     <mergeCell ref="B38:E38"/>
-    <mergeCell ref="B30:E30"/>
-    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="B39:E39"/>
     <mergeCell ref="B31:E31"/>
-    <mergeCell ref="B32:E32"/>
-    <mergeCell ref="B33:E33"/>
-    <mergeCell ref="B34:E34"/>
   </mergeCells>
   <pageMargins left="0.51181102362204722" right="0.51181102362204722" top="0.78740157480314965" bottom="0.78740157480314965" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="97" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
EC1: Correction on SMOTE_Aug_cc32 (IDs 10 and 11 swapped).
</commit_message>
<xml_diff>
--- a/EC1-ECG_Analysis/ecg_oversampling/safetyArtist/Classifiers Conclusions Meanings.xlsx
+++ b/EC1-ECG_Analysis/ecg_oversampling/safetyArtist/Classifiers Conclusions Meanings.xlsx
@@ -70,16 +70,16 @@
     <t>Falsely positive lack of arrithmia expected for the corner case --&gt; truth cat. 1-4, classifier cat. 0 on cc_X0, X non-zero</t>
   </si>
   <si>
-    <t>Falsely positive arrithmia of the expected type for the corner case --&gt; truth = cat. 0, classifier = cat. N on cc_N0, N non-zero</t>
-  </si>
-  <si>
-    <t>Falsely positive arrithmia of an unexpected type for the corner case --&gt; truth = cat. 0, classifier = cat. N on cc_X0, N different from X, N and X non-zero</t>
-  </si>
-  <si>
     <t>Truly positive presence of arrithmia of the expected type for the corner case --&gt; truth = cat. N, classifier cat. X on cc_NX, N different from X, N and X non-zero</t>
   </si>
   <si>
     <t>Truly positive presence of arrithmia of an unexpected type for the corner case --&gt; truth = cat. N, classifier cat. X on cc_NY, N, X and Y all non-zero and mutually different from each other.</t>
+  </si>
+  <si>
+    <t>Falsely positive arrithmia of the expected type for the corner case --&gt; truth = cat. 0, classifier = cat. N on cc_0N, N non-zero</t>
+  </si>
+  <si>
+    <t>Falsely positive arrithmia of an unexpected type for the corner case --&gt; truth = cat. 0, classifier = cat. N on cc_0X, N different from X, N and X non-zero</t>
   </si>
 </sst>
 </file>
@@ -186,17 +186,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -514,7 +514,7 @@
   <dimension ref="A1:E39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -523,12 +523,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="5" t="s">
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="2" t="s">
         <v>9</v>
       </c>
     </row>
@@ -925,7 +925,7 @@
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="5" t="s">
+      <c r="A31" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B31" s="6" t="s">
@@ -939,102 +939,102 @@
       <c r="A32" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B32" s="3" t="s">
+      <c r="B32" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C32" s="3"/>
-      <c r="D32" s="3"/>
-      <c r="E32" s="3"/>
+      <c r="C32" s="4"/>
+      <c r="D32" s="4"/>
+      <c r="E32" s="4"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B33" s="3" t="s">
+      <c r="B33" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C33" s="3"/>
-      <c r="D33" s="3"/>
-      <c r="E33" s="3"/>
+      <c r="C33" s="4"/>
+      <c r="D33" s="4"/>
+      <c r="E33" s="4"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B34" s="2" t="s">
+      <c r="B34" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C34" s="2"/>
-      <c r="D34" s="2"/>
-      <c r="E34" s="2"/>
+      <c r="C34" s="5"/>
+      <c r="D34" s="5"/>
+      <c r="E34" s="5"/>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B35" s="2" t="s">
+      <c r="B35" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C35" s="2"/>
-      <c r="D35" s="2"/>
-      <c r="E35" s="2"/>
+      <c r="C35" s="5"/>
+      <c r="D35" s="5"/>
+      <c r="E35" s="5"/>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B36" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C36" s="2"/>
-      <c r="D36" s="2"/>
-      <c r="E36" s="2"/>
+      <c r="B36" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C36" s="5"/>
+      <c r="D36" s="5"/>
+      <c r="E36" s="5"/>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B37" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C37" s="2"/>
-      <c r="D37" s="2"/>
-      <c r="E37" s="2"/>
+      <c r="B37" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C37" s="5"/>
+      <c r="D37" s="5"/>
+      <c r="E37" s="5"/>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B38" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C38" s="2"/>
-      <c r="D38" s="2"/>
-      <c r="E38" s="2"/>
+      <c r="B38" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C38" s="5"/>
+      <c r="D38" s="5"/>
+      <c r="E38" s="5"/>
     </row>
     <row r="39" spans="1:5" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B39" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C39" s="2"/>
-      <c r="D39" s="2"/>
-      <c r="E39" s="2"/>
+      <c r="B39" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C39" s="5"/>
+      <c r="D39" s="5"/>
+      <c r="E39" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="B36:E36"/>
+    <mergeCell ref="B37:E37"/>
+    <mergeCell ref="B38:E38"/>
+    <mergeCell ref="B39:E39"/>
+    <mergeCell ref="B31:E31"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="B32:E32"/>
     <mergeCell ref="B33:E33"/>
     <mergeCell ref="B34:E34"/>
     <mergeCell ref="B35:E35"/>
-    <mergeCell ref="B36:E36"/>
-    <mergeCell ref="B37:E37"/>
-    <mergeCell ref="B38:E38"/>
-    <mergeCell ref="B39:E39"/>
-    <mergeCell ref="B31:E31"/>
   </mergeCells>
   <pageMargins left="0.51181102362204722" right="0.51181102362204722" top="0.78740157480314965" bottom="0.78740157480314965" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="97" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>